<commit_message>
fix multipicacion EDO assembly
</commit_message>
<xml_diff>
--- a/Fx vs Euler Avanzado.xlsx
+++ b/Fx vs Euler Avanzado.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15340" yWindow="1780" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="20020" yWindow="1480" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -57,9 +60,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1642,7 +1646,7 @@
             <c:numRef>
               <c:f>Hoja1!$C$9:$C$209</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="201"/>
                 <c:pt idx="0">
                   <c:v>0.01</c:v>
@@ -2254,7 +2258,7 @@
             <c:numRef>
               <c:f>Hoja1!$D$9:$D$209</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="201"/>
                 <c:pt idx="0">
                   <c:v>0.999900009999</c:v>
@@ -4484,17 +4488,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C9:H209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="F152" sqref="F152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="9" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>0.01</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <f>1/(C9^2+1)</f>
         <v>0.99990000999900008</v>
       </c>
@@ -4506,10 +4510,10 @@
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>0.02</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <f t="shared" ref="D10:D73" si="0">1/(C10^2+1)</f>
         <v>0.99960015993602558</v>
       </c>
@@ -4521,10 +4525,10 @@
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>0.03</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>0.99910080927165557</v>
       </c>
@@ -4536,10 +4540,10 @@
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>0.04</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>0.99840255591054305</v>
       </c>
@@ -4551,10 +4555,10 @@
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>0.05</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>0.99750623441396513</v>
       </c>
@@ -4566,10 +4570,10 @@
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C14" s="1">
+      <c r="C14" s="2">
         <v>0.06</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>0.99641291351135908</v>
       </c>
@@ -4581,10 +4585,10 @@
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>0.99512389292466918</v>
       </c>
@@ -4596,10 +4600,10 @@
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <v>0.08</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>0.99364069952305245</v>
       </c>
@@ -4611,10 +4615,10 @@
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C17" s="1">
+      <c r="C17" s="2">
         <v>0.09</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>0.99196508282908447</v>
       </c>
@@ -4626,10 +4630,10 @@
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <v>0.1</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>0.99009900990099009</v>
       </c>
@@ -4641,10 +4645,10 @@
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C19" s="1">
+      <c r="C19" s="2">
         <v>0.11</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>0.98804465961861476</v>
       </c>
@@ -4656,10 +4660,10 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C20" s="1">
+      <c r="C20" s="2">
         <v>0.12</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>0.98580441640378547</v>
       </c>
@@ -4671,10 +4675,10 @@
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C21" s="1">
+      <c r="C21" s="2">
         <v>0.13</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>0.98338086340839814</v>
       </c>
@@ -4686,10 +4690,10 @@
       </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C22" s="1">
+      <c r="C22" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>0.98077677520596307</v>
       </c>
@@ -4701,10 +4705,10 @@
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C23" s="1">
+      <c r="C23" s="2">
         <v>0.15</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>0.97799511002444994</v>
       </c>
@@ -4716,10 +4720,10 @@
       </c>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C24" s="1">
+      <c r="C24" s="2">
         <v>0.16</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>0.97503900156006229</v>
       </c>
@@ -4731,10 +4735,10 @@
       </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C25" s="1">
+      <c r="C25" s="2">
         <v>0.17</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>0.97191175041306255</v>
       </c>
@@ -4746,10 +4750,10 @@
       </c>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C26" s="1">
+      <c r="C26" s="2">
         <v>0.18</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="2">
         <f t="shared" si="0"/>
         <v>0.96861681518791165</v>
       </c>
@@ -4761,10 +4765,10 @@
       </c>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C27" s="1">
+      <c r="C27" s="2">
         <v>0.19</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>0.96515780330083967</v>
       </c>
@@ -4776,10 +4780,10 @@
       </c>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C28" s="1">
+      <c r="C28" s="2">
         <v>0.2</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>0.96153846153846145</v>
       </c>
@@ -4791,10 +4795,10 @@
       </c>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C29" s="1">
+      <c r="C29" s="2">
         <v>0.21</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>0.95776266641126329</v>
       </c>
@@ -4806,10 +4810,10 @@
       </c>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C30" s="1">
+      <c r="C30" s="2">
         <v>0.22</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>0.95383441434566962</v>
       </c>
@@ -4821,10 +4825,10 @@
       </c>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C31" s="1">
+      <c r="C31" s="2">
         <v>0.23</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>0.94975781175800178</v>
       </c>
@@ -4836,10 +4840,10 @@
       </c>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C32" s="1">
+      <c r="C32" s="2">
         <v>0.24</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>0.94553706505294999</v>
       </c>
@@ -4851,10 +4855,10 @@
       </c>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C33" s="1">
+      <c r="C33" s="2">
         <v>0.25</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>0.94117647058823528</v>
       </c>
@@ -4866,10 +4870,10 @@
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C34" s="1">
+      <c r="C34" s="2">
         <v>0.26</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>0.93668040464593472</v>
       </c>
@@ -4881,10 +4885,10 @@
       </c>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C35" s="1">
+      <c r="C35" s="2">
         <v>0.27</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>0.93205331344952935</v>
       </c>
@@ -4896,10 +4900,10 @@
       </c>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C36" s="1">
+      <c r="C36" s="2">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="2">
         <f t="shared" si="0"/>
         <v>0.92729970326409494</v>
       </c>
@@ -4911,10 +4915,10 @@
       </c>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C37" s="1">
+      <c r="C37" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="2">
         <f t="shared" si="0"/>
         <v>0.92242413061525685</v>
       </c>
@@ -4926,10 +4930,10 @@
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C38" s="1">
+      <c r="C38" s="2">
         <v>0.3</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="2">
         <f t="shared" si="0"/>
         <v>0.9174311926605504</v>
       </c>
@@ -4941,10 +4945,10 @@
       </c>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C39" s="1">
+      <c r="C39" s="2">
         <v>0.31</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="2">
         <f t="shared" si="0"/>
         <v>0.91232551774473125</v>
       </c>
@@ -4956,10 +4960,10 @@
       </c>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C40" s="1">
+      <c r="C40" s="2">
         <v>0.32</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="2">
         <f t="shared" si="0"/>
         <v>0.90711175616835993</v>
       </c>
@@ -4971,10 +4975,10 @@
       </c>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C41" s="1">
+      <c r="C41" s="2">
         <v>0.33</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41" s="2">
         <f t="shared" si="0"/>
         <v>0.90179457119668138</v>
       </c>
@@ -4986,10 +4990,10 @@
       </c>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C42" s="1">
+      <c r="C42" s="2">
         <v>0.34</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="2">
         <f t="shared" si="0"/>
         <v>0.89637863033345289</v>
       </c>
@@ -5001,10 +5005,10 @@
       </c>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C43" s="1">
+      <c r="C43" s="2">
         <v>0.35</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43" s="2">
         <f t="shared" si="0"/>
         <v>0.89086859688195985</v>
       </c>
@@ -5016,10 +5020,10 @@
       </c>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C44" s="1">
+      <c r="C44" s="2">
         <v>0.36</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44" s="2">
         <f t="shared" si="0"/>
         <v>0.88526912181303119</v>
       </c>
@@ -5031,10 +5035,10 @@
       </c>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C45" s="1">
+      <c r="C45" s="2">
         <v>0.37</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45" s="2">
         <f t="shared" si="0"/>
         <v>0.87958483595742809</v>
       </c>
@@ -5046,10 +5050,10 @@
       </c>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C46" s="1">
+      <c r="C46" s="2">
         <v>0.38</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46" s="2">
         <f t="shared" si="0"/>
         <v>0.87382034253757424</v>
       </c>
@@ -5061,10 +5065,10 @@
       </c>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C47" s="1">
+      <c r="C47" s="2">
         <v>0.39</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D47" s="2">
         <f t="shared" si="0"/>
         <v>0.86798021005121095</v>
       </c>
@@ -5076,10 +5080,10 @@
       </c>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C48" s="1">
+      <c r="C48" s="2">
         <v>0.4</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48" s="2">
         <f t="shared" si="0"/>
         <v>0.86206896551724133</v>
       </c>
@@ -5091,10 +5095,10 @@
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C49" s="1">
+      <c r="C49" s="2">
         <v>0.41</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D49" s="2">
         <f t="shared" si="0"/>
         <v>0.85609108809177303</v>
       </c>
@@ -5106,10 +5110,10 @@
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C50" s="1">
+      <c r="C50" s="2">
         <v>0.42</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50" s="2">
         <f t="shared" si="0"/>
         <v>0.85005100306018366</v>
       </c>
@@ -5121,10 +5125,10 @@
       </c>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C51" s="1">
+      <c r="C51" s="2">
         <v>0.43</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51" s="2">
         <f t="shared" si="0"/>
         <v>0.84395307620896276</v>
       </c>
@@ -5136,10 +5140,10 @@
       </c>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C52" s="1">
+      <c r="C52" s="2">
         <v>0.44</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D52" s="2">
         <f t="shared" si="0"/>
         <v>0.83780160857908847</v>
       </c>
@@ -5151,10 +5155,10 @@
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C53" s="1">
+      <c r="C53" s="2">
         <v>0.45</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D53" s="2">
         <f t="shared" si="0"/>
         <v>0.83160083160083154</v>
       </c>
@@ -5166,10 +5170,10 @@
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C54" s="1">
+      <c r="C54" s="2">
         <v>0.46</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D54" s="2">
         <f t="shared" si="0"/>
         <v>0.8253549026081215</v>
       </c>
@@ -5181,10 +5185,10 @@
       </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C55" s="1">
+      <c r="C55" s="2">
         <v>0.47</v>
       </c>
-      <c r="D55" s="1">
+      <c r="D55" s="2">
         <f t="shared" si="0"/>
         <v>0.81906790072897051</v>
       </c>
@@ -5196,10 +5200,10 @@
       </c>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C56" s="1">
+      <c r="C56" s="2">
         <v>0.48</v>
       </c>
-      <c r="D56" s="1">
+      <c r="D56" s="2">
         <f t="shared" si="0"/>
         <v>0.81274382314694416</v>
       </c>
@@ -5211,10 +5215,10 @@
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C57" s="1">
+      <c r="C57" s="2">
         <v>0.49</v>
       </c>
-      <c r="D57" s="1">
+      <c r="D57" s="2">
         <f t="shared" si="0"/>
         <v>0.80638658172728006</v>
       </c>
@@ -5226,10 +5230,10 @@
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C58" s="1">
+      <c r="C58" s="2">
         <v>0.5</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D58" s="2">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
@@ -5241,10 +5245,10 @@
       </c>
     </row>
     <row r="59" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C59" s="1">
+      <c r="C59" s="2">
         <v>0.51</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D59" s="2">
         <f t="shared" si="0"/>
         <v>0.79358781049123084</v>
       </c>
@@ -5256,10 +5260,10 @@
       </c>
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C60" s="1">
+      <c r="C60" s="2">
         <v>0.52</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D60" s="2">
         <f t="shared" si="0"/>
         <v>0.7871536523929471</v>
       </c>
@@ -5271,10 +5275,10 @@
       </c>
     </row>
     <row r="61" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C61" s="1">
+      <c r="C61" s="2">
         <v>0.53</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D61" s="2">
         <f t="shared" si="0"/>
         <v>0.78070106956046537</v>
       </c>
@@ -5286,10 +5290,10 @@
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C62" s="1">
+      <c r="C62" s="2">
         <v>0.54</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D62" s="2">
         <f t="shared" si="0"/>
         <v>0.77423350882626196</v>
       </c>
@@ -5301,10 +5305,10 @@
       </c>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C63" s="1">
+      <c r="C63" s="2">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D63" s="2">
         <f t="shared" si="0"/>
         <v>0.76775431861804222</v>
       </c>
@@ -5316,10 +5320,10 @@
       </c>
     </row>
     <row r="64" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C64" s="1">
+      <c r="C64" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="D64" s="1">
+      <c r="D64" s="2">
         <f t="shared" si="0"/>
         <v>0.76126674786845305</v>
       </c>
@@ -5331,10 +5335,10 @@
       </c>
     </row>
     <row r="65" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C65" s="1">
+      <c r="C65" s="2">
         <v>0.56999999999999995</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D65" s="2">
         <f t="shared" si="0"/>
         <v>0.75477394520341157</v>
       </c>
@@ -5346,10 +5350,10 @@
       </c>
     </row>
     <row r="66" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C66" s="1">
+      <c r="C66" s="2">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D66" s="2">
         <f t="shared" si="0"/>
         <v>0.74827895839568992</v>
       </c>
@@ -5361,10 +5365,10 @@
       </c>
     </row>
     <row r="67" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C67" s="1">
+      <c r="C67" s="2">
         <v>0.59</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D67" s="2">
         <f t="shared" si="0"/>
         <v>0.74178473407017276</v>
       </c>
@@ -5376,10 +5380,10 @@
       </c>
     </row>
     <row r="68" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C68" s="1">
+      <c r="C68" s="2">
         <v>0.6</v>
       </c>
-      <c r="D68" s="1">
+      <c r="D68" s="2">
         <f t="shared" si="0"/>
         <v>0.73529411764705888</v>
       </c>
@@ -5391,10 +5395,10 @@
       </c>
     </row>
     <row r="69" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C69" s="1">
+      <c r="C69" s="2">
         <v>0.61</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D69" s="2">
         <f t="shared" si="0"/>
         <v>0.72880985350921934</v>
       </c>
@@ -5406,10 +5410,10 @@
       </c>
     </row>
     <row r="70" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C70" s="1">
+      <c r="C70" s="2">
         <v>0.62</v>
       </c>
-      <c r="D70" s="1">
+      <c r="D70" s="2">
         <f t="shared" si="0"/>
         <v>0.72233458537994799</v>
       </c>
@@ -5421,10 +5425,10 @@
       </c>
     </row>
     <row r="71" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C71" s="1">
+      <c r="C71" s="2">
         <v>0.63</v>
       </c>
-      <c r="D71" s="1">
+      <c r="D71" s="2">
         <f t="shared" si="0"/>
         <v>0.7158708568974157</v>
       </c>
@@ -5436,10 +5440,10 @@
       </c>
     </row>
     <row r="72" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C72" s="1">
+      <c r="C72" s="2">
         <v>0.64</v>
       </c>
-      <c r="D72" s="1">
+      <c r="D72" s="2">
         <f t="shared" si="0"/>
         <v>0.70942111237230421</v>
       </c>
@@ -5451,10 +5455,10 @@
       </c>
     </row>
     <row r="73" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C73" s="1">
+      <c r="C73" s="2">
         <v>0.65</v>
       </c>
-      <c r="D73" s="1">
+      <c r="D73" s="2">
         <f t="shared" si="0"/>
         <v>0.70298769771528991</v>
       </c>
@@ -5466,10 +5470,10 @@
       </c>
     </row>
     <row r="74" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C74" s="1">
+      <c r="C74" s="2">
         <v>0.66</v>
       </c>
-      <c r="D74" s="1">
+      <c r="D74" s="2">
         <f t="shared" ref="D74:D137" si="1">1/(C74^2+1)</f>
         <v>0.69657286152131515</v>
       </c>
@@ -5481,10 +5485,10 @@
       </c>
     </row>
     <row r="75" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C75" s="1">
+      <c r="C75" s="2">
         <v>0.67</v>
       </c>
-      <c r="D75" s="1">
+      <c r="D75" s="2">
         <f t="shared" si="1"/>
         <v>0.69017875629788117</v>
       </c>
@@ -5496,10 +5500,10 @@
       </c>
     </row>
     <row r="76" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C76" s="1">
+      <c r="C76" s="2">
         <v>0.68</v>
       </c>
-      <c r="D76" s="1">
+      <c r="D76" s="2">
         <f t="shared" si="1"/>
         <v>0.68380743982494518</v>
       </c>
@@ -5511,10 +5515,10 @@
       </c>
     </row>
     <row r="77" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C77" s="1">
+      <c r="C77" s="2">
         <v>0.69</v>
       </c>
-      <c r="D77" s="1">
+      <c r="D77" s="2">
         <f t="shared" si="1"/>
         <v>0.67746087663437438</v>
       </c>
@@ -5526,10 +5530,10 @@
       </c>
     </row>
     <row r="78" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C78" s="1">
+      <c r="C78" s="2">
         <v>0.7</v>
       </c>
-      <c r="D78" s="1">
+      <c r="D78" s="2">
         <f t="shared" si="1"/>
         <v>0.67114093959731547</v>
       </c>
@@ -5541,10 +5545,10 @@
       </c>
     </row>
     <row r="79" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C79" s="1">
+      <c r="C79" s="2">
         <v>0.71</v>
       </c>
-      <c r="D79" s="1">
+      <c r="D79" s="2">
         <f t="shared" si="1"/>
         <v>0.66484941160827071</v>
       </c>
@@ -5556,10 +5560,10 @@
       </c>
     </row>
     <row r="80" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C80" s="1">
+      <c r="C80" s="2">
         <v>0.72</v>
       </c>
-      <c r="D80" s="1">
+      <c r="D80" s="2">
         <f t="shared" si="1"/>
         <v>0.6585879873551107</v>
       </c>
@@ -5571,10 +5575,10 @@
       </c>
     </row>
     <row r="81" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C81" s="1">
+      <c r="C81" s="2">
         <v>0.73</v>
       </c>
-      <c r="D81" s="1">
+      <c r="D81" s="2">
         <f t="shared" si="1"/>
         <v>0.65235827516472045</v>
       </c>
@@ -5586,10 +5590,10 @@
       </c>
     </row>
     <row r="82" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C82" s="1">
+      <c r="C82" s="2">
         <v>0.74</v>
       </c>
-      <c r="D82" s="1">
+      <c r="D82" s="2">
         <f t="shared" si="1"/>
         <v>0.64616179891444814</v>
       </c>
@@ -5601,10 +5605,10 @@
       </c>
     </row>
     <row r="83" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C83" s="1">
+      <c r="C83" s="2">
         <v>0.75</v>
       </c>
-      <c r="D83" s="1">
+      <c r="D83" s="2">
         <f t="shared" si="1"/>
         <v>0.64</v>
       </c>
@@ -5616,10 +5620,10 @@
       </c>
     </row>
     <row r="84" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C84" s="1">
+      <c r="C84" s="2">
         <v>0.76</v>
       </c>
-      <c r="D84" s="1">
+      <c r="D84" s="2">
         <f t="shared" si="1"/>
         <v>0.6338742393509128</v>
       </c>
@@ -5631,10 +5635,10 @@
       </c>
     </row>
     <row r="85" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C85" s="1">
+      <c r="C85" s="2">
         <v>0.77</v>
       </c>
-      <c r="D85" s="1">
+      <c r="D85" s="2">
         <f t="shared" si="1"/>
         <v>0.62778579948521562</v>
       </c>
@@ -5646,10 +5650,10 @@
       </c>
     </row>
     <row r="86" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C86" s="1">
+      <c r="C86" s="2">
         <v>0.78</v>
       </c>
-      <c r="D86" s="1">
+      <c r="D86" s="2">
         <f t="shared" si="1"/>
         <v>0.62173588659537427</v>
       </c>
@@ -5661,10 +5665,10 @@
       </c>
     </row>
     <row r="87" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C87" s="1">
+      <c r="C87" s="2">
         <v>0.79</v>
       </c>
-      <c r="D87" s="1">
+      <c r="D87" s="2">
         <f t="shared" si="1"/>
         <v>0.61572563265808755</v>
       </c>
@@ -5676,10 +5680,10 @@
       </c>
     </row>
     <row r="88" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C88" s="1">
+      <c r="C88" s="2">
         <v>0.8</v>
       </c>
-      <c r="D88" s="1">
+      <c r="D88" s="2">
         <f t="shared" si="1"/>
         <v>0.6097560975609756</v>
       </c>
@@ -5691,10 +5695,10 @@
       </c>
     </row>
     <row r="89" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C89" s="1">
+      <c r="C89" s="2">
         <v>0.81</v>
       </c>
-      <c r="D89" s="1">
+      <c r="D89" s="2">
         <f t="shared" si="1"/>
         <v>0.60382827123965943</v>
       </c>
@@ -5706,10 +5710,10 @@
       </c>
     </row>
     <row r="90" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C90" s="1">
+      <c r="C90" s="2">
         <v>0.82</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D90" s="2">
         <f t="shared" si="1"/>
         <v>0.59794307581918205</v>
       </c>
@@ -5721,10 +5725,10 @@
       </c>
     </row>
     <row r="91" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C91" s="1">
+      <c r="C91" s="2">
         <v>0.83</v>
       </c>
-      <c r="D91" s="1">
+      <c r="D91" s="2">
         <f t="shared" si="1"/>
         <v>0.59210136775415956</v>
       </c>
@@ -5736,10 +5740,10 @@
       </c>
     </row>
     <row r="92" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C92" s="1">
+      <c r="C92" s="2">
         <v>0.83999900000000005</v>
       </c>
-      <c r="D92" s="1">
+      <c r="D92" s="2">
         <f t="shared" si="1"/>
         <v>0.58630451746658241</v>
       </c>
@@ -5751,10 +5755,10 @@
       </c>
     </row>
     <row r="93" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C93" s="1">
+      <c r="C93" s="2">
         <v>0.84999899999999995</v>
       </c>
-      <c r="D93" s="1">
+      <c r="D93" s="2">
         <f t="shared" si="1"/>
         <v>0.58055209691610121</v>
       </c>
@@ -5766,10 +5770,10 @@
       </c>
     </row>
     <row r="94" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C94" s="1">
+      <c r="C94" s="2">
         <v>0.85999899999999996</v>
       </c>
-      <c r="D94" s="1">
+      <c r="D94" s="2">
         <f t="shared" si="1"/>
         <v>0.57484536027445665</v>
       </c>
@@ -5781,10 +5785,10 @@
       </c>
     </row>
     <row r="95" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C95" s="1">
+      <c r="C95" s="2">
         <v>0.86999899999999997</v>
       </c>
-      <c r="D95" s="1">
+      <c r="D95" s="2">
         <f t="shared" si="1"/>
         <v>0.56918492252330588</v>
       </c>
@@ -5796,10 +5800,10 @@
       </c>
     </row>
     <row r="96" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C96" s="1">
+      <c r="C96" s="2">
         <v>0.87999899999999998</v>
       </c>
-      <c r="D96" s="1">
+      <c r="D96" s="2">
         <f t="shared" si="1"/>
         <v>0.56357134348794014</v>
       </c>
@@ -5811,10 +5815,10 @@
       </c>
     </row>
     <row r="97" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C97" s="1">
+      <c r="C97" s="2">
         <v>0.88999899999999998</v>
       </c>
-      <c r="D97" s="1">
+      <c r="D97" s="2">
         <f t="shared" si="1"/>
         <v>0.5580051298747688</v>
       </c>
@@ -5826,10 +5830,10 @@
       </c>
     </row>
     <row r="98" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C98" s="1">
+      <c r="C98" s="2">
         <v>0.89999899999999999</v>
       </c>
-      <c r="D98" s="1">
+      <c r="D98" s="2">
         <f t="shared" si="1"/>
         <v>0.55248673727932296</v>
       </c>
@@ -5841,10 +5845,10 @@
       </c>
     </row>
     <row r="99" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C99" s="1">
+      <c r="C99" s="2">
         <v>0.909999</v>
       </c>
-      <c r="D99" s="1">
+      <c r="D99" s="2">
         <f t="shared" si="1"/>
         <v>0.54701657216214339</v>
       </c>
@@ -5856,10 +5860,10 @@
       </c>
     </row>
     <row r="100" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C100" s="1">
+      <c r="C100" s="2">
         <v>0.91999900000000001</v>
       </c>
-      <c r="D100" s="1">
+      <c r="D100" s="2">
         <f t="shared" si="1"/>
         <v>0.54159499379021181</v>
       </c>
@@ -5871,10 +5875,10 @@
       </c>
     </row>
     <row r="101" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C101" s="1">
+      <c r="C101" s="2">
         <v>0.92999900000000002</v>
       </c>
-      <c r="D101" s="1">
+      <c r="D101" s="2">
         <f t="shared" si="1"/>
         <v>0.5362223161418691</v>
       </c>
@@ -5886,10 +5890,10 @@
       </c>
     </row>
     <row r="102" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C102" s="1">
+      <c r="C102" s="2">
         <v>0.93999900000000003</v>
       </c>
-      <c r="D102" s="1">
+      <c r="D102" s="2">
         <f t="shared" si="1"/>
         <v>0.5308988097734294</v>
       </c>
@@ -5901,10 +5905,10 @@
       </c>
     </row>
     <row r="103" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C103" s="1">
+      <c r="C103" s="2">
         <v>0.94999900000000004</v>
       </c>
-      <c r="D103" s="1">
+      <c r="D103" s="2">
         <f t="shared" si="1"/>
         <v>0.52562470364594549</v>
       </c>
@@ -5916,10 +5920,10 @@
       </c>
     </row>
     <row r="104" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C104" s="1">
+      <c r="C104" s="2">
         <v>0.95999900000000005</v>
       </c>
-      <c r="D104" s="1">
+      <c r="D104" s="2">
         <f t="shared" si="1"/>
         <v>0.52040018691082357</v>
       </c>
@@ -5931,10 +5935,10 @@
       </c>
     </row>
     <row r="105" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C105" s="1">
+      <c r="C105" s="2">
         <v>0.96999899999999994</v>
       </c>
-      <c r="D105" s="1">
+      <c r="D105" s="2">
         <f t="shared" si="1"/>
         <v>0.51522541065319261</v>
       </c>
@@ -5946,10 +5950,10 @@
       </c>
     </row>
     <row r="106" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C106" s="1">
+      <c r="C106" s="2">
         <v>0.97999899999999995</v>
       </c>
-      <c r="D106" s="1">
+      <c r="D106" s="2">
         <f t="shared" si="1"/>
         <v>0.51010048959214938</v>
       </c>
@@ -5961,10 +5965,10 @@
       </c>
     </row>
     <row r="107" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C107" s="1">
+      <c r="C107" s="2">
         <v>0.98999899999999996</v>
       </c>
-      <c r="D107" s="1">
+      <c r="D107" s="2">
         <f t="shared" si="1"/>
         <v>0.50502550373718114</v>
       </c>
@@ -5976,10 +5980,10 @@
       </c>
     </row>
     <row r="108" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C108" s="1">
+      <c r="C108" s="2">
         <v>0.99999899999999997</v>
       </c>
-      <c r="D108" s="1">
+      <c r="D108" s="2">
         <f t="shared" si="1"/>
         <v>0.50000050000025009</v>
       </c>
@@ -5991,10 +5995,10 @@
       </c>
     </row>
     <row r="109" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C109" s="1">
+      <c r="C109" s="2">
         <v>1.0099990000000001</v>
       </c>
-      <c r="D109" s="1">
+      <c r="D109" s="2">
         <f t="shared" si="1"/>
         <v>0.49502549376318117</v>
       </c>
@@ -6006,10 +6010,10 @@
       </c>
     </row>
     <row r="110" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C110" s="1">
+      <c r="C110" s="2">
         <v>1.0199990000000001</v>
       </c>
-      <c r="D110" s="1">
+      <c r="D110" s="2">
         <f t="shared" si="1"/>
         <v>0.4901004704001517</v>
       </c>
@@ -6021,10 +6025,10 @@
       </c>
     </row>
     <row r="111" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C111" s="1">
+      <c r="C111" s="2">
         <v>1.0299990000000001</v>
       </c>
-      <c r="D111" s="1">
+      <c r="D111" s="2">
         <f t="shared" si="1"/>
         <v>0.48522538675520954</v>
       </c>
@@ -6036,10 +6040,10 @@
       </c>
     </row>
     <row r="112" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C112" s="1">
+      <c r="C112" s="2">
         <v>1.0399989999999999</v>
       </c>
-      <c r="D112" s="1">
+      <c r="D112" s="2">
         <f t="shared" si="1"/>
         <v>0.48040017257488404</v>
       </c>
@@ -6051,10 +6055,10 @@
       </c>
     </row>
     <row r="113" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C113" s="1">
+      <c r="C113" s="2">
         <v>1.0499989999999999</v>
       </c>
-      <c r="D113" s="1">
+      <c r="D113" s="2">
         <f t="shared" si="1"/>
         <v>0.47562473189605781</v>
       </c>
@@ -6066,10 +6070,10 @@
       </c>
     </row>
     <row r="114" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C114" s="1">
+      <c r="C114" s="2">
         <v>1.0599989999999999</v>
       </c>
-      <c r="D114" s="1">
+      <c r="D114" s="2">
         <f t="shared" si="1"/>
         <v>0.47089894438938185</v>
       </c>
@@ -6081,10 +6085,10 @@
       </c>
     </row>
     <row r="115" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C115" s="1">
+      <c r="C115" s="2">
         <v>1.0699989999999999</v>
       </c>
-      <c r="D115" s="1">
+      <c r="D115" s="2">
         <f t="shared" si="1"/>
         <v>0.4662226666586044</v>
       </c>
@@ -6096,10 +6100,10 @@
       </c>
     </row>
     <row r="116" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C116" s="1">
+      <c r="C116" s="2">
         <v>1.0799989999999999</v>
       </c>
-      <c r="D116" s="1">
+      <c r="D116" s="2">
         <f t="shared" si="1"/>
         <v>0.46159573349627164</v>
       </c>
@@ -6111,10 +6115,10 @@
       </c>
     </row>
     <row r="117" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C117" s="1">
+      <c r="C117" s="2">
         <v>1.0899989999999999</v>
       </c>
-      <c r="D117" s="1">
+      <c r="D117" s="2">
         <f t="shared" si="1"/>
         <v>0.45701795909633647</v>
       </c>
@@ -6126,10 +6130,10 @@
       </c>
     </row>
     <row r="118" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C118" s="1">
+      <c r="C118" s="2">
         <v>1.0999989999999999</v>
       </c>
-      <c r="D118" s="1">
+      <c r="D118" s="2">
         <f t="shared" si="1"/>
         <v>0.45248913822427672</v>
       </c>
@@ -6141,10 +6145,10 @@
       </c>
     </row>
     <row r="119" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C119" s="1">
+      <c r="C119" s="2">
         <v>1.109999</v>
       </c>
-      <c r="D119" s="1">
+      <c r="D119" s="2">
         <f t="shared" si="1"/>
         <v>0.44800904734538638</v>
       </c>
@@ -6156,10 +6160,10 @@
       </c>
     </row>
     <row r="120" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C120" s="1">
+      <c r="C120" s="2">
         <v>1.119999</v>
       </c>
-      <c r="D120" s="1">
+      <c r="D120" s="2">
         <f t="shared" si="1"/>
         <v>0.44357744571195656</v>
       </c>
@@ -6171,10 +6175,10 @@
       </c>
     </row>
     <row r="121" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C121" s="1">
+      <c r="C121" s="2">
         <v>1.129999</v>
       </c>
-      <c r="D121" s="1">
+      <c r="D121" s="2">
         <f t="shared" si="1"/>
         <v>0.43919407641010738</v>
       </c>
@@ -6186,10 +6190,10 @@
       </c>
     </row>
     <row r="122" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C122" s="1">
+      <c r="C122" s="2">
         <v>1.139999</v>
       </c>
-      <c r="D122" s="1">
+      <c r="D122" s="2">
         <f t="shared" si="1"/>
         <v>0.43485866736707546</v>
       </c>
@@ -6201,10 +6205,10 @@
       </c>
     </row>
     <row r="123" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C123" s="1">
+      <c r="C123" s="2">
         <v>1.149999</v>
       </c>
-      <c r="D123" s="1">
+      <c r="D123" s="2">
         <f t="shared" si="1"/>
         <v>0.4305709323197906</v>
       </c>
@@ -6216,10 +6220,10 @@
       </c>
     </row>
     <row r="124" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C124" s="1">
+      <c r="C124" s="2">
         <v>1.159999</v>
       </c>
-      <c r="D124" s="1">
+      <c r="D124" s="2">
         <f t="shared" si="1"/>
         <v>0.42633057174560884</v>
       </c>
@@ -6231,10 +6235,10 @@
       </c>
     </row>
     <row r="125" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C125" s="1">
+      <c r="C125" s="2">
         <v>1.169999</v>
       </c>
-      <c r="D125" s="1">
+      <c r="D125" s="2">
         <f t="shared" si="1"/>
         <v>0.42213727375608867</v>
       </c>
@@ -6246,10 +6250,10 @@
       </c>
     </row>
     <row r="126" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C126" s="1">
+      <c r="C126" s="2">
         <v>1.179999</v>
       </c>
-      <c r="D126" s="1">
+      <c r="D126" s="2">
         <f t="shared" si="1"/>
         <v>0.41799071495471879</v>
       </c>
@@ -6261,10 +6265,10 @@
       </c>
     </row>
     <row r="127" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C127" s="1">
+      <c r="C127" s="2">
         <v>1.189999</v>
       </c>
-      <c r="D127" s="1">
+      <c r="D127" s="2">
         <f t="shared" si="1"/>
         <v>0.41389056125951817</v>
       </c>
@@ -6276,10 +6280,10 @@
       </c>
     </row>
     <row r="128" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C128" s="1">
+      <c r="C128" s="2">
         <v>1.199999</v>
       </c>
-      <c r="D128" s="1">
+      <c r="D128" s="2">
         <f t="shared" si="1"/>
         <v>0.40983646869144058</v>
       </c>
@@ -6291,10 +6295,10 @@
       </c>
     </row>
     <row r="129" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C129" s="1">
+      <c r="C129" s="2">
         <v>1.209999</v>
       </c>
-      <c r="D129" s="1">
+      <c r="D129" s="2">
         <f t="shared" si="1"/>
         <v>0.40582808412952309</v>
       </c>
@@ -6306,10 +6310,10 @@
       </c>
     </row>
     <row r="130" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C130" s="1">
+      <c r="C130" s="2">
         <v>1.2199990000000001</v>
       </c>
-      <c r="D130" s="1">
+      <c r="D130" s="2">
         <f t="shared" si="1"/>
         <v>0.40186504603372059</v>
       </c>
@@ -6321,10 +6325,10 @@
       </c>
     </row>
     <row r="131" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C131" s="1">
+      <c r="C131" s="2">
         <v>1.2299990000000001</v>
       </c>
-      <c r="D131" s="1">
+      <c r="D131" s="2">
         <f t="shared" si="1"/>
         <v>0.3979469851363705</v>
       </c>
@@ -6336,10 +6340,10 @@
       </c>
     </row>
     <row r="132" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C132" s="1">
+      <c r="C132" s="2">
         <v>1.2399990000000001</v>
       </c>
-      <c r="D132" s="1">
+      <c r="D132" s="2">
         <f t="shared" si="1"/>
         <v>0.39407352510322669</v>
       </c>
@@ -6351,10 +6355,10 @@
       </c>
     </row>
     <row r="133" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C133" s="1">
+      <c r="C133" s="2">
         <v>1.2499990000000001</v>
       </c>
-      <c r="D133" s="1">
+      <c r="D133" s="2">
         <f t="shared" si="1"/>
         <v>0.39024428316500198</v>
       </c>
@@ -6366,10 +6370,10 @@
       </c>
     </row>
     <row r="134" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C134" s="1">
+      <c r="C134" s="2">
         <v>1.2599990000000001</v>
       </c>
-      <c r="D134" s="1">
+      <c r="D134" s="2">
         <f t="shared" si="1"/>
         <v>0.38645887072034613</v>
       </c>
@@ -6381,10 +6385,10 @@
       </c>
     </row>
     <row r="135" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C135" s="1">
+      <c r="C135" s="2">
         <v>1.2699990000000001</v>
       </c>
-      <c r="D135" s="1">
+      <c r="D135" s="2">
         <f t="shared" si="1"/>
         <v>0.38271689391118213</v>
       </c>
@@ -6396,10 +6400,10 @@
       </c>
     </row>
     <row r="136" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C136" s="1">
+      <c r="C136" s="2">
         <v>1.2799990000000001</v>
       </c>
-      <c r="D136" s="1">
+      <c r="D136" s="2">
         <f t="shared" si="1"/>
         <v>0.37901795417130968</v>
       </c>
@@ -6411,10 +6415,10 @@
       </c>
     </row>
     <row r="137" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C137" s="1">
+      <c r="C137" s="2">
         <v>1.2899989999999999</v>
       </c>
-      <c r="D137" s="1">
+      <c r="D137" s="2">
         <f t="shared" si="1"/>
         <v>0.37536164874917555</v>
       </c>
@@ -6426,10 +6430,10 @@
       </c>
     </row>
     <row r="138" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C138" s="1">
+      <c r="C138" s="2">
         <v>1.2999989999999999</v>
       </c>
-      <c r="D138" s="1">
+      <c r="D138" s="2">
         <f t="shared" ref="D138:D201" si="2">1/(C138^2+1)</f>
         <v>0.37174757120569274</v>
       </c>
@@ -6441,10 +6445,10 @@
       </c>
     </row>
     <row r="139" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C139" s="1">
+      <c r="C139" s="2">
         <v>1.3099989999999999</v>
       </c>
-      <c r="D139" s="1">
+      <c r="D139" s="2">
         <f t="shared" si="2"/>
         <v>0.36817531188798241</v>
       </c>
@@ -6456,10 +6460,10 @@
       </c>
     </row>
     <row r="140" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C140" s="1">
+      <c r="C140" s="2">
         <v>1.3199989999999999</v>
       </c>
-      <c r="D140" s="1">
+      <c r="D140" s="2">
         <f t="shared" si="2"/>
         <v>0.36464445837988824</v>
       </c>
@@ -6471,10 +6475,10 @@
       </c>
     </row>
     <row r="141" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C141" s="1">
+      <c r="C141" s="2">
         <v>1.3299989999999999</v>
       </c>
-      <c r="D141" s="1">
+      <c r="D141" s="2">
         <f t="shared" si="2"/>
         <v>0.36115459593010368</v>
       </c>
@@ -6486,10 +6490,10 @@
       </c>
     </row>
     <row r="142" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C142" s="1">
+      <c r="C142" s="2">
         <v>1.3399989999999999</v>
       </c>
-      <c r="D142" s="1">
+      <c r="D142" s="2">
         <f t="shared" si="2"/>
         <v>0.35770530785873067</v>
       </c>
@@ -6501,10 +6505,10 @@
       </c>
     </row>
     <row r="143" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C143" s="1">
+      <c r="C143" s="2">
         <v>1.3499989999999999</v>
       </c>
-      <c r="D143" s="1">
+      <c r="D143" s="2">
         <f t="shared" si="2"/>
         <v>0.35429617594307206</v>
       </c>
@@ -6516,10 +6520,10 @@
       </c>
     </row>
     <row r="144" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C144" s="1">
+      <c r="C144" s="2">
         <v>1.359999</v>
       </c>
-      <c r="D144" s="1">
+      <c r="D144" s="2">
         <f t="shared" si="2"/>
         <v>0.35092678078344081</v>
       </c>
@@ -6531,10 +6535,10 @@
       </c>
     </row>
     <row r="145" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C145" s="1">
+      <c r="C145" s="2">
         <v>1.369999</v>
       </c>
-      <c r="D145" s="1">
+      <c r="D145" s="2">
         <f t="shared" si="2"/>
         <v>0.34759670214975019</v>
       </c>
@@ -6546,10 +6550,10 @@
       </c>
     </row>
     <row r="146" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C146" s="1">
+      <c r="C146" s="2">
         <v>1.379999</v>
       </c>
-      <c r="D146" s="1">
+      <c r="D146" s="2">
         <f t="shared" si="2"/>
         <v>0.34430551930962988</v>
       </c>
@@ -6561,10 +6565,10 @@
       </c>
     </row>
     <row r="147" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C147" s="1">
+      <c r="C147" s="2">
         <v>1.389999</v>
       </c>
-      <c r="D147" s="1">
+      <c r="D147" s="2">
         <f t="shared" si="2"/>
         <v>0.34105281133879278</v>
       </c>
@@ -6576,10 +6580,10 @@
       </c>
     </row>
     <row r="148" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C148" s="1">
+      <c r="C148" s="2">
         <v>1.399999</v>
       </c>
-      <c r="D148" s="1">
+      <c r="D148" s="2">
         <f t="shared" si="2"/>
         <v>0.33783815741435907</v>
       </c>
@@ -6591,10 +6595,10 @@
       </c>
     </row>
     <row r="149" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C149" s="1">
+      <c r="C149" s="2">
         <v>1.409999</v>
       </c>
-      <c r="D149" s="1">
+      <c r="D149" s="2">
         <f t="shared" si="2"/>
         <v>0.33466113709182155</v>
       </c>
@@ -6606,10 +6610,10 @@
       </c>
     </row>
     <row r="150" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C150" s="1">
+      <c r="C150" s="2">
         <v>1.419999</v>
       </c>
-      <c r="D150" s="1">
+      <c r="D150" s="2">
         <f t="shared" si="2"/>
         <v>0.33152133056631988</v>
       </c>
@@ -6621,10 +6625,10 @@
       </c>
     </row>
     <row r="151" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C151" s="1">
+      <c r="C151" s="2">
         <v>1.429999</v>
       </c>
-      <c r="D151" s="1">
+      <c r="D151" s="2">
         <f t="shared" si="2"/>
         <v>0.32841831891886886</v>
       </c>
@@ -6636,10 +6640,10 @@
       </c>
     </row>
     <row r="152" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C152" s="1">
+      <c r="C152" s="2">
         <v>1.439999</v>
       </c>
-      <c r="D152" s="1">
+      <c r="D152" s="2">
         <f t="shared" si="2"/>
         <v>0.3253516843481668</v>
       </c>
@@ -6651,10 +6655,10 @@
       </c>
     </row>
     <row r="153" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C153" s="1">
+      <c r="C153" s="2">
         <v>1.449999</v>
       </c>
-      <c r="D153" s="1">
+      <c r="D153" s="2">
         <f t="shared" si="2"/>
         <v>0.32232101038859234</v>
       </c>
@@ -6666,10 +6670,10 @@
       </c>
     </row>
     <row r="154" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C154" s="1">
+      <c r="C154" s="2">
         <v>1.459999</v>
       </c>
-      <c r="D154" s="1">
+      <c r="D154" s="2">
         <f t="shared" si="2"/>
         <v>0.3193258821149752</v>
       </c>
@@ -6681,10 +6685,10 @@
       </c>
     </row>
     <row r="155" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C155" s="1">
+      <c r="C155" s="2">
         <v>1.4699990000000001</v>
       </c>
-      <c r="D155" s="1">
+      <c r="D155" s="2">
         <f t="shared" si="2"/>
         <v>0.31636588633471147</v>
       </c>
@@ -6696,10 +6700,10 @@
       </c>
     </row>
     <row r="156" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C156" s="1">
+      <c r="C156" s="2">
         <v>1.4799990000000001</v>
       </c>
-      <c r="D156" s="1">
+      <c r="D156" s="2">
         <f t="shared" si="2"/>
         <v>0.31344061176777122</v>
       </c>
@@ -6711,10 +6715,10 @@
       </c>
     </row>
     <row r="157" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C157" s="1">
+      <c r="C157" s="2">
         <v>1.4899990000000001</v>
       </c>
-      <c r="D157" s="1">
+      <c r="D157" s="2">
         <f t="shared" si="2"/>
         <v>0.31054964921513123</v>
       </c>
@@ -6726,10 +6730,10 @@
       </c>
     </row>
     <row r="158" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C158" s="1">
+      <c r="C158" s="2">
         <v>1.4999990000000001</v>
       </c>
-      <c r="D158" s="1">
+      <c r="D158" s="2">
         <f t="shared" si="2"/>
         <v>0.30769259171614383</v>
       </c>
@@ -6741,10 +6745,10 @@
       </c>
     </row>
     <row r="159" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C159" s="1">
+      <c r="C159" s="2">
         <v>1.5099990000000001</v>
       </c>
-      <c r="D159" s="1">
+      <c r="D159" s="2">
         <f t="shared" si="2"/>
         <v>0.30486903469533849</v>
       </c>
@@ -6756,10 +6760,10 @@
       </c>
     </row>
     <row r="160" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C160" s="1">
+      <c r="C160" s="2">
         <v>1.5199990000000001</v>
       </c>
-      <c r="D160" s="1">
+      <c r="D160" s="2">
         <f t="shared" si="2"/>
         <v>0.3020785760991328</v>
       </c>
@@ -6771,10 +6775,10 @@
       </c>
     </row>
     <row r="161" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C161" s="1">
+      <c r="C161" s="2">
         <v>1.5299990000000001</v>
       </c>
-      <c r="D161" s="1">
+      <c r="D161" s="2">
         <f t="shared" si="2"/>
         <v>0.2993208165229127</v>
       </c>
@@ -6786,10 +6790,10 @@
       </c>
     </row>
     <row r="162" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C162" s="1">
+      <c r="C162" s="2">
         <v>1.5399989999999999</v>
       </c>
-      <c r="D162" s="1">
+      <c r="D162" s="2">
         <f t="shared" si="2"/>
         <v>0.296595359328927</v>
       </c>
@@ -6801,10 +6805,10 @@
       </c>
     </row>
     <row r="163" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C163" s="1">
+      <c r="C163" s="2">
         <v>1.5499989999999999</v>
       </c>
-      <c r="D163" s="1">
+      <c r="D163" s="2">
         <f t="shared" si="2"/>
         <v>0.29390181075542088</v>
       </c>
@@ -6816,10 +6820,10 @@
       </c>
     </row>
     <row r="164" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C164" s="1">
+      <c r="C164" s="2">
         <v>1.5599989999999999</v>
       </c>
-      <c r="D164" s="1">
+      <c r="D164" s="2">
         <f t="shared" si="2"/>
         <v>0.29123978001742268</v>
       </c>
@@ -6831,10 +6835,10 @@
       </c>
     </row>
     <row r="165" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C165" s="1">
+      <c r="C165" s="2">
         <v>1.5699989999999999</v>
       </c>
-      <c r="D165" s="1">
+      <c r="D165" s="2">
         <f t="shared" si="2"/>
         <v>0.28860887939957652</v>
       </c>
@@ -6846,10 +6850,10 @@
       </c>
     </row>
     <row r="166" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C166" s="1">
+      <c r="C166" s="2">
         <v>1.5799989999999999</v>
       </c>
-      <c r="D166" s="1">
+      <c r="D166" s="2">
         <f t="shared" si="2"/>
         <v>0.28600872434140345</v>
       </c>
@@ -6861,10 +6865,10 @@
       </c>
     </row>
     <row r="167" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C167" s="1">
+      <c r="C167" s="2">
         <v>1.5899989999999999</v>
       </c>
-      <c r="D167" s="1">
+      <c r="D167" s="2">
         <f t="shared" si="2"/>
         <v>0.28343893351535537</v>
       </c>
@@ -6876,10 +6880,10 @@
       </c>
     </row>
     <row r="168" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C168" s="1">
+      <c r="C168" s="2">
         <v>1.5999989999999999</v>
       </c>
-      <c r="D168" s="1">
+      <c r="D168" s="2">
         <f t="shared" si="2"/>
         <v>0.28089912889801449</v>
       </c>
@@ -6891,10 +6895,10 @@
       </c>
     </row>
     <row r="169" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C169" s="1">
+      <c r="C169" s="2">
         <v>1.609999</v>
       </c>
-      <c r="D169" s="1">
+      <c r="D169" s="2">
         <f t="shared" si="2"/>
         <v>0.27838893583477492</v>
       </c>
@@ -6906,10 +6910,10 @@
       </c>
     </row>
     <row r="170" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C170" s="1">
+      <c r="C170" s="2">
         <v>1.619999</v>
       </c>
-      <c r="D170" s="1">
+      <c r="D170" s="2">
         <f t="shared" si="2"/>
         <v>0.27590798309833059</v>
       </c>
@@ -6921,10 +6925,10 @@
       </c>
     </row>
     <row r="171" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C171" s="1">
+      <c r="C171" s="2">
         <v>1.629999</v>
       </c>
-      <c r="D171" s="1">
+      <c r="D171" s="2">
         <f t="shared" si="2"/>
         <v>0.27345590294128092</v>
       </c>
@@ -6936,10 +6940,10 @@
       </c>
     </row>
     <row r="172" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C172" s="1">
+      <c r="C172" s="2">
         <v>1.639999</v>
       </c>
-      <c r="D172" s="1">
+      <c r="D172" s="2">
         <f t="shared" si="2"/>
         <v>0.27103233114315239</v>
       </c>
@@ -6951,10 +6955,10 @@
       </c>
     </row>
     <row r="173" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C173" s="1">
+      <c r="C173" s="2">
         <v>1.649999</v>
       </c>
-      <c r="D173" s="1">
+      <c r="D173" s="2">
         <f t="shared" si="2"/>
         <v>0.26863690705212212</v>
       </c>
@@ -6966,10 +6970,10 @@
       </c>
     </row>
     <row r="174" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C174" s="1">
+      <c r="C174" s="2">
         <v>1.659999</v>
       </c>
-      <c r="D174" s="1">
+      <c r="D174" s="2">
         <f t="shared" si="2"/>
         <v>0.26626927362171748</v>
       </c>
@@ -6981,10 +6985,10 @@
       </c>
     </row>
     <row r="175" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C175" s="1">
+      <c r="C175" s="2">
         <v>1.669999</v>
       </c>
-      <c r="D175" s="1">
+      <c r="D175" s="2">
         <f t="shared" si="2"/>
         <v>0.26392907744275507</v>
       </c>
@@ -6996,10 +7000,10 @@
       </c>
     </row>
     <row r="176" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C176" s="1">
+      <c r="C176" s="2">
         <v>1.679999</v>
       </c>
-      <c r="D176" s="1">
+      <c r="D176" s="2">
         <f t="shared" si="2"/>
         <v>0.26161596877077059</v>
       </c>
@@ -7011,10 +7015,10 @@
       </c>
     </row>
     <row r="177" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C177" s="1">
+      <c r="C177" s="2">
         <v>1.689999</v>
       </c>
-      <c r="D177" s="1">
+      <c r="D177" s="2">
         <f t="shared" si="2"/>
         <v>0.25932960154918022</v>
       </c>
@@ -7026,10 +7030,10 @@
       </c>
     </row>
     <row r="178" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C178" s="1">
+      <c r="C178" s="2">
         <v>1.699999</v>
       </c>
-      <c r="D178" s="1">
+      <c r="D178" s="2">
         <f t="shared" si="2"/>
         <v>0.25706963342840528</v>
       </c>
@@ -7041,10 +7045,10 @@
       </c>
     </row>
     <row r="179" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C179" s="1">
+      <c r="C179" s="2">
         <v>1.709999</v>
       </c>
-      <c r="D179" s="1">
+      <c r="D179" s="2">
         <f t="shared" si="2"/>
         <v>0.25483572578117969</v>
       </c>
@@ -7056,10 +7060,10 @@
       </c>
     </row>
     <row r="180" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C180" s="1">
+      <c r="C180" s="2">
         <v>1.7199990000000001</v>
       </c>
-      <c r="D180" s="1">
+      <c r="D180" s="2">
         <f t="shared" si="2"/>
         <v>0.25262754371425267</v>
       </c>
@@ -7071,10 +7075,10 @@
       </c>
     </row>
     <row r="181" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C181" s="1">
+      <c r="C181" s="2">
         <v>1.7299990000000001</v>
       </c>
-      <c r="D181" s="1">
+      <c r="D181" s="2">
         <f t="shared" si="2"/>
         <v>0.25044475607668748</v>
       </c>
@@ -7086,10 +7090,10 @@
       </c>
     </row>
     <row r="182" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C182" s="1">
+      <c r="C182" s="2">
         <v>1.7399990000000001</v>
       </c>
-      <c r="D182" s="1">
+      <c r="D182" s="2">
         <f t="shared" si="2"/>
         <v>0.2482870354649506</v>
       </c>
@@ -7101,10 +7105,10 @@
       </c>
     </row>
     <row r="183" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C183" s="1">
+      <c r="C183" s="2">
         <v>1.7499990000000001</v>
       </c>
-      <c r="D183" s="1">
+      <c r="D183" s="2">
         <f t="shared" si="2"/>
         <v>0.24615405822497419</v>
       </c>
@@ -7116,10 +7120,10 @@
       </c>
     </row>
     <row r="184" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C184" s="1">
+      <c r="C184" s="2">
         <v>1.7599990000000001</v>
       </c>
-      <c r="D184" s="1">
+      <c r="D184" s="2">
         <f t="shared" si="2"/>
         <v>0.24404550445136949</v>
       </c>
@@ -7131,10 +7135,10 @@
       </c>
     </row>
     <row r="185" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C185" s="1">
+      <c r="C185" s="2">
         <v>1.7699990000000001</v>
       </c>
-      <c r="D185" s="1">
+      <c r="D185" s="2">
         <f t="shared" si="2"/>
         <v>0.24196105798395875</v>
       </c>
@@ -7146,10 +7150,10 @@
       </c>
     </row>
     <row r="186" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C186" s="1">
+      <c r="C186" s="2">
         <v>1.7799990000000001</v>
       </c>
-      <c r="D186" s="1">
+      <c r="D186" s="2">
         <f t="shared" si="2"/>
         <v>0.23990040640178648</v>
       </c>
@@ -7161,10 +7165,10 @@
       </c>
     </row>
     <row r="187" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C187" s="1">
+      <c r="C187" s="2">
         <v>1.7899989999999999</v>
       </c>
-      <c r="D187" s="1">
+      <c r="D187" s="2">
         <f t="shared" si="2"/>
         <v>0.237863241014763</v>
       </c>
@@ -7176,10 +7180,10 @@
       </c>
     </row>
     <row r="188" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C188" s="1">
+      <c r="C188" s="2">
         <v>1.7999989999999999</v>
       </c>
-      <c r="D188" s="1">
+      <c r="D188" s="2">
         <f t="shared" si="2"/>
         <v>0.23584925685308702</v>
       </c>
@@ -7191,10 +7195,10 @@
       </c>
     </row>
     <row r="189" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C189" s="1">
+      <c r="C189" s="2">
         <v>1.8099989999999999</v>
       </c>
-      <c r="D189" s="1">
+      <c r="D189" s="2">
         <f t="shared" si="2"/>
         <v>0.23385815265458682</v>
       </c>
@@ -7206,10 +7210,10 @@
       </c>
     </row>
     <row r="190" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C190" s="1">
+      <c r="C190" s="2">
         <v>1.8199989999999999</v>
       </c>
-      <c r="D190" s="1">
+      <c r="D190" s="2">
         <f t="shared" si="2"/>
         <v>0.23188963085011235</v>
       </c>
@@ -7221,10 +7225,10 @@
       </c>
     </row>
     <row r="191" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C191" s="1">
+      <c r="C191" s="2">
         <v>1.8299989999999999</v>
       </c>
-      <c r="D191" s="1">
+      <c r="D191" s="2">
         <f t="shared" si="2"/>
         <v>0.22994339754710505</v>
       </c>
@@ -7236,10 +7240,10 @@
       </c>
     </row>
     <row r="192" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C192" s="1">
+      <c r="C192" s="2">
         <v>1.8399989999999999</v>
       </c>
-      <c r="D192" s="1">
+      <c r="D192" s="2">
         <f t="shared" si="2"/>
         <v>0.22801916251146712</v>
       </c>
@@ -7251,10 +7255,10 @@
       </c>
     </row>
     <row r="193" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C193" s="1">
+      <c r="C193" s="2">
         <v>1.8499989999999999</v>
       </c>
-      <c r="D193" s="1">
+      <c r="D193" s="2">
         <f t="shared" si="2"/>
         <v>0.22611663914784369</v>
       </c>
@@ -7266,10 +7270,10 @@
       </c>
     </row>
     <row r="194" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C194" s="1">
+      <c r="C194" s="2">
         <v>1.859999</v>
       </c>
-      <c r="D194" s="1">
+      <c r="D194" s="2">
         <f t="shared" si="2"/>
         <v>0.22423554447842886</v>
       </c>
@@ -7281,10 +7285,10 @@
       </c>
     </row>
     <row r="195" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C195" s="1">
+      <c r="C195" s="2">
         <v>1.869999</v>
       </c>
-      <c r="D195" s="1">
+      <c r="D195" s="2">
         <f t="shared" si="2"/>
         <v>0.22237559912039814</v>
       </c>
@@ -7296,10 +7300,10 @@
       </c>
     </row>
     <row r="196" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C196" s="1">
+      <c r="C196" s="2">
         <v>1.879999</v>
       </c>
-      <c r="D196" s="1">
+      <c r="D196" s="2">
         <f t="shared" si="2"/>
         <v>0.22053652726206821</v>
       </c>
@@ -7311,10 +7315,10 @@
       </c>
     </row>
     <row r="197" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C197" s="1">
+      <c r="C197" s="2">
         <v>1.889999</v>
       </c>
-      <c r="D197" s="1">
+      <c r="D197" s="2">
         <f t="shared" si="2"/>
         <v>0.21871805663787655</v>
       </c>
@@ -7326,10 +7330,10 @@
       </c>
     </row>
     <row r="198" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C198" s="1">
+      <c r="C198" s="2">
         <v>1.899999</v>
       </c>
-      <c r="D198" s="1">
+      <c r="D198" s="2">
         <f t="shared" si="2"/>
         <v>0.21691991850227191</v>
       </c>
@@ -7341,10 +7345,10 @@
       </c>
     </row>
     <row r="199" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C199" s="1">
+      <c r="C199" s="2">
         <v>1.909999</v>
       </c>
-      <c r="D199" s="1">
+      <c r="D199" s="2">
         <f t="shared" si="2"/>
         <v>0.2151418476025995</v>
       </c>
@@ -7356,10 +7360,10 @@
       </c>
     </row>
     <row r="200" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C200" s="1">
+      <c r="C200" s="2">
         <v>1.919999</v>
       </c>
-      <c r="D200" s="1">
+      <c r="D200" s="2">
         <f t="shared" si="2"/>
         <v>0.21338358215106309</v>
       </c>
@@ -7371,10 +7375,10 @@
       </c>
     </row>
     <row r="201" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C201" s="1">
+      <c r="C201" s="2">
         <v>1.929999</v>
       </c>
-      <c r="D201" s="1">
+      <c r="D201" s="2">
         <f t="shared" si="2"/>
         <v>0.21164486379583961</v>
       </c>
@@ -7386,10 +7390,10 @@
       </c>
     </row>
     <row r="202" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C202" s="1">
+      <c r="C202" s="2">
         <v>1.939999</v>
       </c>
-      <c r="D202" s="1">
+      <c r="D202" s="2">
         <f t="shared" ref="D202:D209" si="3">1/(C202^2+1)</f>
         <v>0.20992543759141993</v>
       </c>
@@ -7401,10 +7405,10 @@
       </c>
     </row>
     <row r="203" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C203" s="1">
+      <c r="C203" s="2">
         <v>1.9499979999999999</v>
       </c>
-      <c r="D203" s="1">
+      <c r="D203" s="2">
         <f t="shared" si="3"/>
         <v>0.20822522106317365</v>
       </c>
@@ -7416,10 +7420,10 @@
       </c>
     </row>
     <row r="204" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C204" s="1">
+      <c r="C204" s="2">
         <v>1.9599979999999999</v>
       </c>
-      <c r="D204" s="1">
+      <c r="D204" s="2">
         <f t="shared" si="3"/>
         <v>0.20654362592969291</v>
       </c>
@@ -7431,10 +7435,10 @@
       </c>
     </row>
     <row r="205" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C205" s="1">
+      <c r="C205" s="2">
         <v>1.9699979999999999</v>
       </c>
-      <c r="D205" s="1">
+      <c r="D205" s="2">
         <f t="shared" si="3"/>
         <v>0.20488057826592171</v>
       </c>
@@ -7446,10 +7450,10 @@
       </c>
     </row>
     <row r="206" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C206" s="1">
+      <c r="C206" s="2">
         <v>1.9799979999999999</v>
       </c>
-      <c r="D206" s="1">
+      <c r="D206" s="2">
         <f t="shared" si="3"/>
         <v>0.20323583644155185</v>
       </c>
@@ -7461,10 +7465,10 @@
       </c>
     </row>
     <row r="207" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C207" s="1">
+      <c r="C207" s="2">
         <v>1.9899979999999999</v>
       </c>
-      <c r="D207" s="1">
+      <c r="D207" s="2">
         <f t="shared" si="3"/>
         <v>0.20160916207498311</v>
       </c>
@@ -7476,10 +7480,10 @@
       </c>
     </row>
     <row r="208" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C208" s="1">
+      <c r="C208" s="2">
         <v>1.9999979999999999</v>
       </c>
-      <c r="D208" s="1">
+      <c r="D208" s="2">
         <f t="shared" si="3"/>
         <v>0.20000032000035203</v>
       </c>
@@ -7491,10 +7495,10 @@
       </c>
     </row>
     <row r="209" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C209" s="1">
+      <c r="C209" s="2">
         <v>2.0099990000000001</v>
       </c>
-      <c r="D209" s="1">
+      <c r="D209" s="2">
         <f t="shared" si="3"/>
         <v>0.19840891998247254</v>
       </c>

</xml_diff>